<commit_message>
Update role selection question text and remove formatting symbols
</commit_message>
<xml_diff>
--- a/data/hag.xlsx
+++ b/data/hag.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDSko\Desktop\DevAI\HayAutoGrade\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9385A174-D7AA-4B7E-AFC4-9068BB445537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F098ED02-11DA-4457-AB84-C4344057C682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,9 +759,6 @@
   </si>
   <si>
     <t>варианты ответов на 12 вопрос</t>
-  </si>
-  <si>
-    <t>Укажите точное название должности, которую мы оцениваем</t>
   </si>
   <si>
     <t>Сформулируйте главную цель этой роли. Какую основную ценность она создает для организации?</t>
@@ -1837,6 +1834,9 @@
 Отвечайте, пожалуйста, исходя из реальных требований и сложности роли, а не из качеств конкретного сотрудника
 В примерах к каждому вопросу приведены ориентиры для одной условной должности — «Менеджер по продажам». Используйте их как образец стиля ответа, а не как точный шаблон. Ваша задача — описать именно ту роль, которую вы оцениваете</t>
   </si>
+  <si>
+    <t>Выберите роль для оценки в структуре компании</t>
+  </si>
 </sst>
 </file>
 
@@ -2518,7 +2518,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2553,10 +2553,10 @@
         <v>25</v>
       </c>
       <c r="G1" s="39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2564,16 +2564,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>176</v>
+        <v>269</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="123.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2581,16 +2581,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="131" customHeight="1" x14ac:dyDescent="0.35">
@@ -2598,16 +2598,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2615,16 +2615,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>243</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
@@ -2632,14 +2632,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="6"/>
       <c r="G6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -2648,16 +2648,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>246</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2665,16 +2665,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>248</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2682,19 +2682,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2702,19 +2702,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2722,19 +2722,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2742,21 +2742,21 @@
         <v>11</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E12" s="33" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="110.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2764,21 +2764,21 @@
         <v>12</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E13" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2786,19 +2786,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2806,10 +2806,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>262</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>18</v>
@@ -2818,10 +2818,10 @@
         <v>23</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2829,10 +2829,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>19</v>
@@ -2841,10 +2841,10 @@
         <v>24</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="343.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2852,19 +2852,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -2872,14 +2872,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="6"/>
       <c r="G18" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H18" s="3"/>
     </row>
@@ -2888,16 +2888,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>268</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -19830,7 +19830,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="116" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -19858,13 +19858,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -20194,7 +20194,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -20205,7 +20205,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -20216,7 +20216,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -20227,7 +20227,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -20238,7 +20238,7 @@
         <v>5</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -20249,7 +20249,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I36" s="3"/>
     </row>
@@ -20261,7 +20261,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -20272,7 +20272,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -20283,7 +20283,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -20294,7 +20294,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -20305,7 +20305,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -20316,7 +20316,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -20327,7 +20327,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -20338,7 +20338,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -20349,7 +20349,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -20360,7 +20360,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -20371,7 +20371,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="41" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -20382,7 +20382,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -20393,7 +20393,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -20404,7 +20404,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -20415,7 +20415,7 @@
         <v>6</v>
       </c>
       <c r="C51" s="41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -20426,7 +20426,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -20437,7 +20437,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files and telegram bot
</commit_message>
<xml_diff>
--- a/data/hag.xlsx
+++ b/data/hag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDSko\Desktop\DevAI\HayAutoGrade\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F098ED02-11DA-4457-AB84-C4344057C682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4D402B-2FEE-4568-8791-3A2DF8AD7F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="563" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -1829,13 +1829,12 @@
 Например: "Функционал - это конкретные задачи, которые вы выполняете. Например: 'ведение CRM', 'переговоры с клиентами', 'подготовка отчетов'. Опишите ваши основные функции."</t>
   </si>
   <si>
-    <t>Вводное пояснение для пользователя:
-Добрый день! Этот опрос поможет оценить уровень позиции в вашей команде по международной методике HAY Group. 
+    <t>Выберите роль для оценки в структуре компании</t>
+  </si>
+  <si>
+    <t>Добрый день! Этот опрос поможет оценить уровень позиции в вашей команде по международной методике HAY Group. 
 Отвечайте, пожалуйста, исходя из реальных требований и сложности роли, а не из качеств конкретного сотрудника
 В примерах к каждому вопросу приведены ориентиры для одной условной должности — «Менеджер по продажам». Используйте их как образец стиля ответа, а не как точный шаблон. Ваша задача — описать именно ту роль, которую вы оцениваете</t>
-  </si>
-  <si>
-    <t>Выберите роль для оценки в структуре компании</t>
   </si>
 </sst>
 </file>
@@ -2517,7 +2516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2564,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>238</v>
@@ -19819,8 +19818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CFE3D3-6274-4674-A955-E380785831A1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19828,9 +19827,9 @@
     <col min="1" max="1" width="96.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update hag.xlsx with formatted examples
</commit_message>
<xml_diff>
--- a/data/hag.xlsx
+++ b/data/hag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDSko\Desktop\DevAI\HayAutoGrade\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9491442-6720-4061-A2E0-DAC76AFA09D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C5D472-E9FF-465C-93BE-F388945F96E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="563" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -764,10 +764,6 @@
     <t>Сформулируйте главную цель этой роли. Какую основную ценность она создает для организации?</t>
   </si>
   <si>
-    <t>Опишите полную иерархию структурных подразделений, к которым относится эта роль, начиная с высшего уровня. Требуется указать минимум два уровня. Перечисляйте подразделения через запятую, от высшего к низшему.
-Пример: Департамент информационных технологий, Управление разработки, Отдел бэкенд-разработки</t>
-  </si>
-  <si>
     <t>"
 {user_answer}
 Проанализируй диалог и определи, назвал ли пользователь конкретную должность.
@@ -1271,32 +1267,6 @@
     <t>вспомогательный текст для столбца инструкция_проверки</t>
   </si>
   <si>
-    <t>Ты ведешь диалог с пользователем, чтобы узнать точное название должности, которую оцениваем.
-{dialog}
-АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
-- Учитывай все ответы пользователя, не только последний
-- Не задавай вопросы повторно
-- После 2-3 уточнений будь готов принять ответ
-ПРИНИМАЙ ответ, если понятно, какая конкретная должность имеется в виду:
-✓ "Менеджер по продажам"
-✓ "Frontend-разработчик"
-✓ "Главный бухгалтер"
-✓ "Менеджер"
-✓ "Аналитик"
-НЕ ПРИНИМАЙ слишком общие формулировки:
-✗ "Работник"
-✗ "Сотрудник"
-✗ "Человек который продает"
-✗ "Не знаю"
-ФОРМАТ ОТВЕТА:
-- Если название должности понятно → пиши: "ПРИНЯТО"
-- Если нужно уточнение → задай короткий конкретный вопрос (БЕЗ префикса "УТОЧНИ:")
-  Например: "Уточните, пожалуйста, конкретное название должности. Например: 'Менеджер по продажам' или 'Главный бухгалтер'."
-ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
-Ответь кратко. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
-Например: "Должность - это название позиции, например: 'Менеджер по продажам', 'Программист', 'Бухгалтер'. Какая должность у вас?"</t>
-  </si>
-  <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать главную цель роли и ценность для организации.
 {dialog}
 АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
@@ -1324,39 +1294,6 @@
 Например: "Цель роли - это то, зачем нужна должность. Например: 'привлечение клиентов', 'обеспечение качества'. Расскажите о цели вашей роли?"</t>
   </si>
   <si>
-    <t>Ты ведешь диалог с пользователем, чтобы узнать иерархию структурных подразделений (минимум 2 уровня).
-{dialog}
-АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
-- Учитывай все ответы пользователя, не только последний
-- Не задавай вопросы повторно
-- После 2-3 уточнений будь готов принять ответ
-ОБЯЗАТЕЛЬНОЕ ТРЕБОВАНИЕ: Минимум ДВА уровня подразделений.
-Один уровень недопустим (это уровень генерального директора).
-ПРИНИМАЙ ответ, если указана иерархия из 2+ уровней:
-✓ "Коммерческий блок / Департамент продаж"
-✓ "IT-дирекция / Отдел разработки / Группа frontend"
-✓ "Финансовый блок / Бухгалтерия"
-✓ "Производственное подразделение / Цех №1"
-Принимай любой формат разделителей: "/", "&gt;", "-", "→" или текст "входит в", "подчиняется".
-НЕ ПРИНИМАЙ:
-✗ Только ОДИН уровень (недопустимо)
-✗ "Не знаю"
-✗ "Прямое подчинение директору"
-✗ Полностью не по теме
-ФОРМАТ ОТВЕТА:
-- Если указано минимум 2 уровня → пиши: "ПРИНЯТО"
-- Если указан только 1 уровень → объясни, что это уровень генерального директора, попроси указать более детальную структуру
-- Если нужно уточнение → задай короткий конкретный вопрос (БЕЗ префикса "УТОЧНИ:")
-  Например: "Укажите, пожалуйста, минимум два уровня. Например: 'IT-дирекция / Отдел разработки'."
-ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
-Кратко ответь, попроси указать структуру. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
-Например: "Структурные подразделения - это иерархия отделов. Например: 'IT-дирекция / Отдел разработки'. Укажите минимум 2 уровня для вашей должности."</t>
-  </si>
-  <si>
-    <t>Назовите должность непосредственного руководителя для оцениваемой роли
-Пример: начальник отдела продаж</t>
-  </si>
-  <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать точную должность непосредственного руководителя.
 {dialog}
 АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
@@ -1382,14 +1319,6 @@
 ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
 Кратко ответь и попроси указать должность. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
 Например: "Укажите должность вашего непосредственного руководителя, например: 'Начальник отдела продаж' или 'Директор департамента'."</t>
-  </si>
-  <si>
-    <t>Какое минимальное образование необходимо для этой роли?
-Пример: среднее специальное или высшее неполное</t>
-  </si>
-  <si>
-    <t>Нужно ли дополнительное профильное образование? Если да, укажите программы и статус (обязательные/рекомендуемые).
-Пример: курсы по технике продаж — рекомендуемые</t>
   </si>
   <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать требуется ли дополнительное профильное образование.
@@ -1421,10 +1350,6 @@
 ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
 Кратко ответь и попроси дать развернутый ответ. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
 Например: "Дополнительное образование - это курсы, сертификации, программы повышения квалификации. Требуется ли что-то подобное для вашей должности?"</t>
-  </si>
-  <si>
-    <t>Какие знания и навыки требуются? Укажите важные языки (если нужны), профессиональные и технические умения, а также другие ключевые требования.
-Пример: свободное владение русским﻿ и английским (B2)﻿, базовые навыки работы с CRM</t>
   </si>
   <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать специализированные знания и навыки по категориям: Языки, Отраслевые знания, Технические навыки, Другие требования.
@@ -1465,10 +1390,6 @@
 Например: "Укажите требования по категориям: языки, отраслевые знания (финансы, IT и др.), технические навыки (ПО, инструменты), другие требования. Что требуется для вашей должности?"</t>
   </si>
   <si>
-    <t>Опишите взаимодействие с людьми: с кем, цель, частота.
-Пример: общение с клиентами для заключения сделок, ежедневно</t>
-  </si>
-  <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать уровень взаимодействия с людьми, требуемый для должности.
 {dialog}
 АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
@@ -1496,10 +1417,6 @@
 Например: "Опишите, с кем и как происходит взаимодействие: базовое общение и обмен информацией, убеждение и переговоры, или мотивация и управление людьми?"</t>
   </si>
   <si>
-    <t>Опишите уровень планирования: сроки, задачи, контроль, самостоятельность.
-Пример: планирует ежемесячные цели по продажам, самостоятельно выбирает методы работы</t>
-  </si>
-  <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать уровень планирования и организации для роли.
 {dialog}
 АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
@@ -1525,10 +1442,6 @@
 ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
 Кратко ответь и попроси описать задачи. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
 Например: "Опишите характер ваших задач: выполнение конкретных операций, координация с коллегами, планирование работы отдела или управление несколькими направлениями?"</t>
-  </si>
-  <si>
-    <t>Какой уровень знаний и опыта требуется?
-Пример: опыт продаж от 1 года, базовые навыки переговоров</t>
   </si>
   <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать уровень экспертизы и глубины знаний, требуемый для должности.
@@ -1559,10 +1472,6 @@
 Например: "Опишите требуемый уровень экспертизы: базовые навыки с обучением на месте, специализированное образование и опыт, или глубокая экспертиза с многолетним опытом?"</t>
   </si>
   <si>
-    <t>Насколько свободно принимаются решения?
-Пример: самостоятельно выбирает способы привлечения клиентов и проводит переговоры</t>
-  </si>
-  <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать степень свободы мышления, требуемую для решения задач на должности.
 {dialog}
 АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
@@ -1589,10 +1498,6 @@
 ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
 Кратко ответь и попроси описать степень свободы. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
 Например: "Опишите уровень самостоятельности: работа по строгим инструкциям, выбор из готовых вариантов, оптимизация процессов или разработка собственных методов работы?"</t>
-  </si>
-  <si>
-    <t>Как часто требуются нестандартные решения?
-Пример: регулярно, для адаптации под клиента</t>
   </si>
   <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать уровень креативности и оригинальности мышления, требуемый для должности.
@@ -1622,10 +1527,6 @@
 Например: "Опишите, как часто нужны нестандартные решения: работа по инструкции, выбор из готовых методов, адаптация подходов или создание новых концепций?"</t>
   </si>
   <si>
-    <t>Можно ли измерить результат работы в деньгах? Если да, укажите пример метрики.
-Пример: план по продажам — 10 млн рублей в квартал</t>
-  </si>
-  <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать можно ли оценить результат деятельности в денежном выражении за год.
 {dialog}
 АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
@@ -1653,10 +1554,6 @@
 ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
 Кратко ответь и попроси описать возможность оценки. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
 Например: "Можно ли измерить результат вашей работы в деньгах? Например: план продаж, бюджет, экономия затрат. Если нельзя - так и укажите."</t>
-  </si>
-  <si>
-    <t>Опишите масштаб влияния: на какие процессы или подразделения влияет роль?
-Пример: влияет на доходы отдела продаж и общий коммерческий результат</t>
   </si>
   <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать степень влияния должности на конечные результаты компании.
@@ -1715,10 +1612,6 @@
 Например: "Опишите масштаб влияния: разовые поручения, работа внутри отдела, участие в ключевых процессах компании, аналитика и рекомендации или руководство командами?"</t>
   </si>
   <si>
-    <t>Опишите степень полномочий при принятии решений.
-Пример: принимает решения о скидках в рамках утверждённой политики</t>
-  </si>
-  <si>
     <t>Ты ведешь диалог с пользователем, чтобы узнать степень полномочий при принятии решений для должности.
 {dialog}
 АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
@@ -1746,10 +1639,6 @@
 ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
 Кратко ответь и попроси описать полномочия. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
 Например: "Опишите степень полномочий: постоянный контроль, работа по инструкциям с выбором порядка действий, частичная самостоятельность или полная ответственность за результаты?"</t>
-  </si>
-  <si>
-    <t>Как организован контроль результатов работы? Кто и с какой частотой оценивает?
-Пример: контроль руководителем отдела еженедельно</t>
   </si>
   <si>
     <t>Укажите основные функции и задачи оцениваемой роли</t>
@@ -1782,9 +1671,6 @@
 ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
 Кратко ответь и попроси описать функционал. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
 Например: "Функционал - это конкретные задачи, которые вы выполняете. Например: 'ведение CRM', 'переговоры с клиентами', 'подготовка отчетов'. Опишите ваши основные функции."</t>
-  </si>
-  <si>
-    <t>Выберите роль для оценки в структуре компании</t>
   </si>
   <si>
     <t>Добрый день! Этот опрос поможет оценить уровень позиции в вашей команде по международной методике HAY Group. 
@@ -1835,6 +1721,96 @@
   </si>
   <si>
     <t>VI. Воздействующее</t>
+  </si>
+  <si>
+    <t>Укажите точное название должности, которую мы оцениваем</t>
+  </si>
+  <si>
+    <t>Сколько уровней (CEO-1, CEO-2, CEO-3 и т.д.) отделяют сотрудника от генерального директора?</t>
+  </si>
+  <si>
+    <t>CEO-1;CEO-2;CEO-3;CEO-4;CEO-5 и более</t>
+  </si>
+  <si>
+    <t>Ты ведешь диалог с пользователем, чтобы узнать точное название должности, которую оцениваем.
+{dialog}
+АНАЛИЗИРУЙ ВСЮ ИСТОРИЮ ДИАЛОГА:
+- Учитывай все ответы пользователя, не только последний
+- Не задавай вопросы повторно
+- После 2-3 уточнений будь готов принять ответ
+ПРИНИМАЙ ответ, если понятно, какая конкретная должность имеется в виду:
+✓ "Менеджер по продажам"
+✓ "Frontend-разработчик"
+✓ "Главный бухгалтер"
+✓ "Менеджер"
+✓ "Аналитик"
+✓ "Руководитель направления"
+✓ "Руководитель проектов"
+✓ "Директор проектов"
+НЕ ПРИНИМАЙ слишком общие формулировки:
+✗ "Работник"
+✗ "Сотрудник"
+✗ "Человек который продает"
+✗ "Не знаю"
+ФОРМАТ ОТВЕТА:
+- Если название должности понятно → пиши: "ПРИНЯТО"
+- Если нужно уточнение → задай короткий конкретный вопрос (БЕЗ префикса "УТОЧНИ:")
+  Например: "Уточните, пожалуйста, конкретное название должности. Например: 'Менеджер по продажам' или 'Главный бухгалтер'."
+ЕСЛИ ПОЛЬЗОВАТЕЛЬ ЗАДАЕТ ВОПРОС:
+Ответь кратко. Если пользователь просит привести пример, приводи его на основе любой другой максимально простой должности, не схожей с той, которая сейчас оценивается. Не подстраивай пример под возможный профиль пользователя
+Например: "Должность - это название позиции, например: 'Менеджер по продажам', 'Программист', 'Бухгалтер'. Какая должность у вас?"</t>
+  </si>
+  <si>
+    <t>Назовите должность непосредственного руководителя для оцениваемой роли
+Например, для менеджера по продажам: начальник отдела продаж</t>
+  </si>
+  <si>
+    <t>Какое минимальное образование необходимо для этой роли?
+Например, для менеджера по продажам: среднее специальное или высшее неполное</t>
+  </si>
+  <si>
+    <t>Нужно ли дополнительное профильное образование? Если да, укажите программы и статус (обязательные/рекомендуемые).
+Например, для менеджера по продажам: курсы по технике продаж — рекомендуемые</t>
+  </si>
+  <si>
+    <t>Какие знания и навыки требуются? Укажите важные языки (если нужны), профессиональные и технические умения, а также другие ключевые требования.
+Например, для менеджера по продажам: свободное владение русским﻿ и английским (B2)﻿, базовые навыки работы с CRM</t>
+  </si>
+  <si>
+    <t>Опишите взаимодействие с людьми: с кем, цель, частота.
+Например, для менеджера по продажам: общение с клиентами для заключения сделок, ежедневно</t>
+  </si>
+  <si>
+    <t>Опишите уровень планирования: сроки, задачи, контроль, самостоятельность.
+Например, для менеджера по продажам: планирует ежемесячные цели по продажам, самостоятельно выбирает методы работы</t>
+  </si>
+  <si>
+    <t>Какой уровень знаний и опыта требуется?
+Например, для менеджера по продажам: опыт продаж от 1 года, базовые навыки переговоров</t>
+  </si>
+  <si>
+    <t>Насколько свободно принимаются решения?
+Например, для менеджера по продажам: самостоятельно выбирает способы привлечения клиентов и проводит переговоры</t>
+  </si>
+  <si>
+    <t>Как часто требуются нестандартные решения?
+Например, для менеджера по продажам: регулярно, для адаптации под клиента</t>
+  </si>
+  <si>
+    <t>Можно ли измерить результат работы в деньгах? Если да, укажите пример метрики.
+Например, для менеджера по продажам: план по продажам — 10 млн рублей в квартал</t>
+  </si>
+  <si>
+    <t>Опишите масштаб влияния: на какие процессы или подразделения влияет роль?
+Например, для менеджера по продажам: влияет на доходы отдела продаж и общий коммерческий результат</t>
+  </si>
+  <si>
+    <t>Опишите степень полномочий при принятии решений.
+Например, для менеджера по продажам: принимает решения о скидках в рамках утверждённой политики</t>
+  </si>
+  <si>
+    <t>Как организован контроль результатов работы? Кто и с какой частотой оценивает?
+Например, для менеджера по продажам: контроль руководителем отдела еженедельно</t>
   </si>
 </sst>
 </file>
@@ -2516,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2552,10 +2528,10 @@
         <v>25</v>
       </c>
       <c r="G1" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2566,25 +2542,26 @@
         <v>253</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>223</v>
+        <v>256</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="123.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="131" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>224</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" s="6"/>
       <c r="G3" s="1" t="s">
         <v>208</v>
       </c>
@@ -2592,21 +2569,21 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="131" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="123.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2614,16 +2591,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
@@ -2631,14 +2608,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="6"/>
       <c r="G6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -2647,16 +2624,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2664,16 +2641,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>231</v>
+        <v>260</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2681,19 +2658,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2701,19 +2678,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2721,19 +2698,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2741,21 +2718,21 @@
         <v>11</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="6" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="E12" s="33" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="110.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2763,21 +2740,21 @@
         <v>12</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="6" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="E13" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2785,19 +2762,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>243</v>
+        <v>266</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2805,10 +2782,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>18</v>
@@ -2817,10 +2794,10 @@
         <v>23</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -2828,10 +2805,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>19</v>
@@ -2840,10 +2817,10 @@
         <v>24</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="343.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2851,34 +2828,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="6"/>
       <c r="G18" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H18" s="3"/>
     </row>
@@ -2887,16 +2864,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -19829,7 +19806,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -19841,7 +19818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49D5B3B-4CF0-40E5-A45D-13ED7B1921AB}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:C53"/>
     </sheetView>
   </sheetViews>
@@ -19857,13 +19834,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -20193,7 +20170,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -20204,7 +20181,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -20215,7 +20192,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -20226,7 +20203,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -20237,7 +20214,7 @@
         <v>5</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -20248,7 +20225,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="I36" s="3"/>
     </row>
@@ -20260,7 +20237,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -20271,7 +20248,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -20282,7 +20259,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -20293,7 +20270,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -20304,7 +20281,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -20315,7 +20292,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -20326,7 +20303,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -20337,7 +20314,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -20348,7 +20325,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -20359,7 +20336,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -20370,7 +20347,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -20381,7 +20358,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -20392,7 +20369,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -20403,7 +20380,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -20414,7 +20391,7 @@
         <v>6</v>
       </c>
       <c r="C51" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -20425,7 +20402,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -20436,7 +20413,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update hag.xlsx final version
</commit_message>
<xml_diff>
--- a/data/hag.xlsx
+++ b/data/hag.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDSko\Desktop\DevAI\HayAutoGrade\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C5D472-E9FF-465C-93BE-F388945F96E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2543C7-3480-43BA-90F6-61DA21DB75D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1777,10 +1777,6 @@
 Например, для менеджера по продажам: свободное владение русским﻿ и английским (B2)﻿, базовые навыки работы с CRM</t>
   </si>
   <si>
-    <t>Опишите взаимодействие с людьми: с кем, цель, частота.
-Например, для менеджера по продажам: общение с клиентами для заключения сделок, ежедневно</t>
-  </si>
-  <si>
     <t>Опишите уровень планирования: сроки, задачи, контроль, самостоятельность.
 Например, для менеджера по продажам: планирует ежемесячные цели по продажам, самостоятельно выбирает методы работы</t>
   </si>
@@ -1811,6 +1807,10 @@
   <si>
     <t>Как организован контроль результатов работы? Кто и с какой частотой оценивает?
 Например, для менеджера по продажам: контроль руководителем отдела еженедельно</t>
+  </si>
+  <si>
+    <t>С кем будет взаимодействовать данная роль? Как часто и с какой целью?
+Например, для менеджера по продажам: общение с клиентами для заключения сделок, ежедневно</t>
   </si>
 </sst>
 </file>
@@ -2492,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2658,7 +2658,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>226</v>
@@ -2678,7 +2678,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>227</v>
@@ -2698,7 +2698,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>228</v>
@@ -2718,7 +2718,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="6" t="s">
@@ -2740,7 +2740,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="6" t="s">
@@ -2762,7 +2762,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>231</v>
@@ -2782,7 +2782,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>232</v>
@@ -2805,7 +2805,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>233</v>
@@ -2828,7 +2828,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>234</v>
@@ -2848,7 +2848,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>22</v>

</xml_diff>